<commit_message>
upd: final to protecting
</commit_message>
<xml_diff>
--- a/Setup/BillTemplate.xlsx
+++ b/Setup/BillTemplate.xlsx
@@ -309,7 +309,6 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -328,33 +327,30 @@
     <xf numFmtId="164" fontId="3" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,7 +637,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,18 +645,18 @@
     <col min="1" max="1" width="23.140625" customWidth="1"/>
     <col min="2" max="2" width="0.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="26.85546875" customWidth="1"/>
-    <col min="4" max="4" width="1.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="0.7109375" style="2" customWidth="1"/>
     <col min="5" max="7" width="3.85546875" customWidth="1"/>
     <col min="8" max="8" width="7.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="33" x14ac:dyDescent="0.45">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="22"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="25"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -668,12 +664,12 @@
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="26"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -682,9 +678,9 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-      <c r="B3" s="17"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="8"/>
-      <c r="D3" s="32"/>
+      <c r="D3" s="24"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
@@ -693,11 +689,11 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="27" t="s">
+      <c r="B4" s="16"/>
+      <c r="C4" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="30"/>
+      <c r="D4" s="22"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="8"/>
@@ -705,14 +701,14 @@
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="17"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="30"/>
+      <c r="D5" s="22"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
@@ -720,12 +716,12 @@
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="30"/>
+      <c r="D6" s="22"/>
       <c r="E6" s="3"/>
       <c r="F6" s="6"/>
       <c r="G6" s="8"/>
@@ -733,12 +729,12 @@
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="30"/>
+      <c r="D7" s="22"/>
       <c r="E7" s="3"/>
       <c r="F7" s="6"/>
       <c r="G7" s="8"/>
@@ -746,12 +742,12 @@
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="30"/>
+      <c r="D8" s="22"/>
       <c r="E8" s="3"/>
       <c r="F8" s="6"/>
       <c r="G8" s="8"/>
@@ -762,7 +758,7 @@
       <c r="A9" s="9"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="30"/>
+      <c r="D9" s="22"/>
       <c r="E9" s="3"/>
       <c r="F9" s="6"/>
       <c r="G9" s="8"/>
@@ -770,12 +766,12 @@
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="30"/>
+      <c r="D10" s="22"/>
       <c r="E10" s="3"/>
       <c r="F10" s="6"/>
       <c r="G10" s="8"/>
@@ -783,12 +779,12 @@
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="14" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="30"/>
+      <c r="D11" s="22"/>
       <c r="E11" s="3"/>
       <c r="F11" s="6"/>
       <c r="G11" s="8"/>
@@ -796,25 +792,25 @@
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="30"/>
+      <c r="D12" s="22"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
       <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="15" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="30"/>
+      <c r="D13" s="22"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -825,7 +821,7 @@
       <c r="A14" s="10"/>
       <c r="B14" s="3"/>
       <c r="C14" s="6"/>
-      <c r="D14" s="30"/>
+      <c r="D14" s="22"/>
       <c r="E14" s="6"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -833,12 +829,12 @@
       <c r="I14" s="4"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="6"/>
-      <c r="D15" s="30"/>
+      <c r="D15" s="22"/>
       <c r="E15" s="6"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -846,12 +842,12 @@
       <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="19">
+      <c r="A16" s="18">
         <v>123456789</v>
       </c>
-      <c r="B16" s="28"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="30"/>
+      <c r="D16" s="22"/>
       <c r="E16" s="6"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -859,12 +855,12 @@
       <c r="I16" s="4"/>
     </row>
     <row r="17" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="31"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="23"/>
       <c r="E17" s="6"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -879,10 +875,10 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
   </mergeCells>
-  <pageMargins left="7.874015748031496E-2" right="0" top="7.874015748031496E-2" bottom="7.874015748031496E-2" header="0" footer="0"/>
-  <pageSetup paperSize="258" scale="87" fitToWidth="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
+  <pageMargins left="0.47244094488188981" right="0.62992125984251968" top="0.39370078740157483" bottom="0.39370078740157483" header="0.19685039370078741" footer="0.19685039370078741"/>
+  <pageSetup paperSize="258" scale="73" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>